<commit_message>
Refreshing dates in tutorial spreadsheet
</commit_message>
<xml_diff>
--- a/docs/tutorials/on-call-rotation.xlsx
+++ b/docs/tutorials/on-call-rotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23612"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34B908E-756E-4368-BFC1-6259492AE8B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C310C0E8-66D1-4807-B444-B8B28BFB5CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +202,11 @@
       <color rgb="FFF2F2F2"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -225,13 +230,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +630,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -643,18 +648,18 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -664,10 +669,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>44200</v>
+        <v>44565</v>
       </c>
       <c r="D3" s="2">
-        <v>44207</v>
+        <v>44572</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
@@ -678,10 +683,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="2">
-        <v>44207</v>
+        <v>44572</v>
       </c>
       <c r="D4" s="2">
-        <v>44214</v>
+        <v>44579</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
@@ -692,10 +697,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="2">
-        <v>44214</v>
+        <v>44579</v>
       </c>
       <c r="D5" s="2">
-        <v>44221</v>
+        <v>44586</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
@@ -706,10 +711,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>44221</v>
+        <v>44586</v>
       </c>
       <c r="D6" s="2">
-        <v>44228</v>
+        <v>44593</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
@@ -720,10 +725,10 @@
         <v>13</v>
       </c>
       <c r="C7" s="2">
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="D7" s="2">
-        <v>44235</v>
+        <v>44600</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
@@ -734,10 +739,10 @@
         <v>15</v>
       </c>
       <c r="C8" s="2">
-        <v>44235</v>
+        <v>44600</v>
       </c>
       <c r="D8" s="2">
-        <v>44242</v>
+        <v>44607</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
@@ -748,12 +753,12 @@
         <v>17</v>
       </c>
       <c r="C9" s="2">
-        <v>44242</v>
+        <v>44607</v>
       </c>
       <c r="D9" s="2">
-        <v>44249</v>
-      </c>
-      <c r="I9" s="7" t="s">
+        <v>44614</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -765,10 +770,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="2">
-        <v>44249</v>
+        <v>44614</v>
       </c>
       <c r="D10" s="2">
-        <v>44256</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
@@ -779,10 +784,10 @@
         <v>22</v>
       </c>
       <c r="C11" s="2">
-        <v>44256</v>
+        <v>44621</v>
       </c>
       <c r="D11" s="3">
-        <v>44263</v>
+        <v>44628</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
@@ -793,10 +798,10 @@
         <v>24</v>
       </c>
       <c r="C12" s="3">
-        <v>44263</v>
+        <v>44628</v>
       </c>
       <c r="D12" s="2">
-        <v>44270</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
@@ -807,12 +812,12 @@
         <v>26</v>
       </c>
       <c r="C13" s="2">
-        <v>44270</v>
+        <v>44635</v>
       </c>
       <c r="D13" s="2">
-        <v>44277</v>
-      </c>
-      <c r="L13" s="7"/>
+        <v>44642</v>
+      </c>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
@@ -822,10 +827,10 @@
         <v>28</v>
       </c>
       <c r="C14" s="2">
-        <v>44277</v>
+        <v>44642</v>
       </c>
       <c r="D14" s="2">
-        <v>44284</v>
+        <v>44649</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
@@ -836,10 +841,10 @@
         <v>30</v>
       </c>
       <c r="C15" s="2">
-        <v>44284</v>
+        <v>44649</v>
       </c>
       <c r="D15" s="2">
-        <v>44291</v>
+        <v>44656</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
@@ -850,10 +855,10 @@
         <v>32</v>
       </c>
       <c r="C16" s="2">
-        <v>44291</v>
+        <v>44656</v>
       </c>
       <c r="D16" s="2">
-        <v>44298</v>
+        <v>44663</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -864,10 +869,10 @@
         <v>34</v>
       </c>
       <c r="C17" s="2">
-        <v>44298</v>
+        <v>44663</v>
       </c>
       <c r="D17" s="2">
-        <v>44305</v>
+        <v>44670</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -878,10 +883,10 @@
         <v>36</v>
       </c>
       <c r="C18" s="2">
-        <v>44305</v>
+        <v>44670</v>
       </c>
       <c r="D18" s="2">
-        <v>44312</v>
+        <v>44677</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
@@ -892,10 +897,10 @@
         <v>38</v>
       </c>
       <c r="C19" s="2">
-        <v>44312</v>
+        <v>44677</v>
       </c>
       <c r="D19" s="2">
-        <v>44319</v>
+        <v>44684</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -906,10 +911,10 @@
         <v>40</v>
       </c>
       <c r="C20" s="2">
-        <v>44319</v>
+        <v>44684</v>
       </c>
       <c r="D20" s="3">
-        <v>44326</v>
+        <v>44691</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -920,10 +925,10 @@
         <v>42</v>
       </c>
       <c r="C21" s="3">
-        <v>44326</v>
+        <v>44691</v>
       </c>
       <c r="D21" s="2">
-        <v>44333</v>
+        <v>44698</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
@@ -934,10 +939,10 @@
         <v>44</v>
       </c>
       <c r="C22" s="2">
-        <v>44333</v>
+        <v>44698</v>
       </c>
       <c r="D22" s="2">
-        <v>44341</v>
+        <v>44706</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
@@ -948,10 +953,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="2">
-        <v>44341</v>
+        <v>44706</v>
       </c>
       <c r="D23" s="2">
-        <v>44207</v>
+        <v>44572</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
@@ -962,10 +967,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="2">
-        <v>44347</v>
+        <v>44712</v>
       </c>
       <c r="D24" s="2">
-        <v>44214</v>
+        <v>44579</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
@@ -976,10 +981,10 @@
         <v>9</v>
       </c>
       <c r="C25" s="2">
-        <v>44354</v>
+        <v>44719</v>
       </c>
       <c r="D25" s="2">
-        <v>44361</v>
+        <v>44726</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
@@ -990,10 +995,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="2">
-        <v>44361</v>
+        <v>44726</v>
       </c>
       <c r="D26" s="2">
-        <v>44368</v>
+        <v>44733</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
@@ -1004,10 +1009,10 @@
         <v>13</v>
       </c>
       <c r="C27" s="2">
-        <v>44368</v>
+        <v>44733</v>
       </c>
       <c r="D27" s="2">
-        <v>44375</v>
+        <v>44740</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
@@ -1018,10 +1023,10 @@
         <v>15</v>
       </c>
       <c r="C28" s="2">
-        <v>44375</v>
+        <v>44740</v>
       </c>
       <c r="D28" s="2">
-        <v>44382</v>
+        <v>44747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refreshing dates in tutorial spreadsheet (#483)
</commit_message>
<xml_diff>
--- a/docs/tutorials/on-call-rotation.xlsx
+++ b/docs/tutorials/on-call-rotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23612"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\tutorials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34B908E-756E-4368-BFC1-6259492AE8B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C310C0E8-66D1-4807-B444-B8B28BFB5CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +202,11 @@
       <color rgb="FFF2F2F2"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -225,13 +230,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +630,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -643,18 +648,18 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -664,10 +669,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>44200</v>
+        <v>44565</v>
       </c>
       <c r="D3" s="2">
-        <v>44207</v>
+        <v>44572</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
@@ -678,10 +683,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="2">
-        <v>44207</v>
+        <v>44572</v>
       </c>
       <c r="D4" s="2">
-        <v>44214</v>
+        <v>44579</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
@@ -692,10 +697,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="2">
-        <v>44214</v>
+        <v>44579</v>
       </c>
       <c r="D5" s="2">
-        <v>44221</v>
+        <v>44586</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
@@ -706,10 +711,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>44221</v>
+        <v>44586</v>
       </c>
       <c r="D6" s="2">
-        <v>44228</v>
+        <v>44593</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
@@ -720,10 +725,10 @@
         <v>13</v>
       </c>
       <c r="C7" s="2">
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="D7" s="2">
-        <v>44235</v>
+        <v>44600</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
@@ -734,10 +739,10 @@
         <v>15</v>
       </c>
       <c r="C8" s="2">
-        <v>44235</v>
+        <v>44600</v>
       </c>
       <c r="D8" s="2">
-        <v>44242</v>
+        <v>44607</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
@@ -748,12 +753,12 @@
         <v>17</v>
       </c>
       <c r="C9" s="2">
-        <v>44242</v>
+        <v>44607</v>
       </c>
       <c r="D9" s="2">
-        <v>44249</v>
-      </c>
-      <c r="I9" s="7" t="s">
+        <v>44614</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -765,10 +770,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="2">
-        <v>44249</v>
+        <v>44614</v>
       </c>
       <c r="D10" s="2">
-        <v>44256</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
@@ -779,10 +784,10 @@
         <v>22</v>
       </c>
       <c r="C11" s="2">
-        <v>44256</v>
+        <v>44621</v>
       </c>
       <c r="D11" s="3">
-        <v>44263</v>
+        <v>44628</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
@@ -793,10 +798,10 @@
         <v>24</v>
       </c>
       <c r="C12" s="3">
-        <v>44263</v>
+        <v>44628</v>
       </c>
       <c r="D12" s="2">
-        <v>44270</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
@@ -807,12 +812,12 @@
         <v>26</v>
       </c>
       <c r="C13" s="2">
-        <v>44270</v>
+        <v>44635</v>
       </c>
       <c r="D13" s="2">
-        <v>44277</v>
-      </c>
-      <c r="L13" s="7"/>
+        <v>44642</v>
+      </c>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
@@ -822,10 +827,10 @@
         <v>28</v>
       </c>
       <c r="C14" s="2">
-        <v>44277</v>
+        <v>44642</v>
       </c>
       <c r="D14" s="2">
-        <v>44284</v>
+        <v>44649</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.45">
@@ -836,10 +841,10 @@
         <v>30</v>
       </c>
       <c r="C15" s="2">
-        <v>44284</v>
+        <v>44649</v>
       </c>
       <c r="D15" s="2">
-        <v>44291</v>
+        <v>44656</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
@@ -850,10 +855,10 @@
         <v>32</v>
       </c>
       <c r="C16" s="2">
-        <v>44291</v>
+        <v>44656</v>
       </c>
       <c r="D16" s="2">
-        <v>44298</v>
+        <v>44663</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -864,10 +869,10 @@
         <v>34</v>
       </c>
       <c r="C17" s="2">
-        <v>44298</v>
+        <v>44663</v>
       </c>
       <c r="D17" s="2">
-        <v>44305</v>
+        <v>44670</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -878,10 +883,10 @@
         <v>36</v>
       </c>
       <c r="C18" s="2">
-        <v>44305</v>
+        <v>44670</v>
       </c>
       <c r="D18" s="2">
-        <v>44312</v>
+        <v>44677</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
@@ -892,10 +897,10 @@
         <v>38</v>
       </c>
       <c r="C19" s="2">
-        <v>44312</v>
+        <v>44677</v>
       </c>
       <c r="D19" s="2">
-        <v>44319</v>
+        <v>44684</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -906,10 +911,10 @@
         <v>40</v>
       </c>
       <c r="C20" s="2">
-        <v>44319</v>
+        <v>44684</v>
       </c>
       <c r="D20" s="3">
-        <v>44326</v>
+        <v>44691</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -920,10 +925,10 @@
         <v>42</v>
       </c>
       <c r="C21" s="3">
-        <v>44326</v>
+        <v>44691</v>
       </c>
       <c r="D21" s="2">
-        <v>44333</v>
+        <v>44698</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
@@ -934,10 +939,10 @@
         <v>44</v>
       </c>
       <c r="C22" s="2">
-        <v>44333</v>
+        <v>44698</v>
       </c>
       <c r="D22" s="2">
-        <v>44341</v>
+        <v>44706</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
@@ -948,10 +953,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="2">
-        <v>44341</v>
+        <v>44706</v>
       </c>
       <c r="D23" s="2">
-        <v>44207</v>
+        <v>44572</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
@@ -962,10 +967,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="2">
-        <v>44347</v>
+        <v>44712</v>
       </c>
       <c r="D24" s="2">
-        <v>44214</v>
+        <v>44579</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
@@ -976,10 +981,10 @@
         <v>9</v>
       </c>
       <c r="C25" s="2">
-        <v>44354</v>
+        <v>44719</v>
       </c>
       <c r="D25" s="2">
-        <v>44361</v>
+        <v>44726</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
@@ -990,10 +995,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="2">
-        <v>44361</v>
+        <v>44726</v>
       </c>
       <c r="D26" s="2">
-        <v>44368</v>
+        <v>44733</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
@@ -1004,10 +1009,10 @@
         <v>13</v>
       </c>
       <c r="C27" s="2">
-        <v>44368</v>
+        <v>44733</v>
       </c>
       <c r="D27" s="2">
-        <v>44375</v>
+        <v>44740</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
@@ -1018,10 +1023,10 @@
         <v>15</v>
       </c>
       <c r="C28" s="2">
-        <v>44375</v>
+        <v>44740</v>
       </c>
       <c r="D28" s="2">
-        <v>44382</v>
+        <v>44747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updatng tutorials and some samples
</commit_message>
<xml_diff>
--- a/docs/tutorials/on-call-rotation.xlsx
+++ b/docs/tutorials/on-call-rotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\tutorials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint-df.com/personal/aljerabe_microsoft_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C310C0E8-66D1-4807-B444-B8B28BFB5CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{C310C0E8-66D1-4807-B444-B8B28BFB5CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E976836-2AF3-4976-98C4-F30870386028}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1" sheetId="1" r:id="rId1"/>
@@ -331,9 +331,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,7 +371,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -477,7 +477,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -630,18 +630,18 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -655,13 +655,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -669,13 +669,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>44565</v>
+        <v>45295</v>
       </c>
       <c r="D3" s="2">
-        <v>44572</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -683,13 +683,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="2">
-        <v>44572</v>
+        <v>45302</v>
       </c>
       <c r="D4" s="2">
-        <v>44579</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -697,13 +697,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="2">
-        <v>44579</v>
+        <v>45309</v>
       </c>
       <c r="D5" s="2">
-        <v>44586</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -711,13 +711,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>44586</v>
+        <v>45316</v>
       </c>
       <c r="D6" s="2">
-        <v>44593</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -725,13 +725,13 @@
         <v>13</v>
       </c>
       <c r="C7" s="2">
-        <v>44593</v>
+        <v>45323</v>
       </c>
       <c r="D7" s="2">
-        <v>44600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -739,13 +739,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="2">
-        <v>44600</v>
+        <v>45330</v>
       </c>
       <c r="D8" s="2">
-        <v>44607</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -753,16 +753,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="2">
-        <v>44607</v>
+        <v>45337</v>
       </c>
       <c r="D9" s="2">
-        <v>44614</v>
+        <v>45344</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -770,13 +770,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="2">
-        <v>44614</v>
+        <v>45344</v>
       </c>
       <c r="D10" s="2">
-        <v>44621</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -784,13 +784,13 @@
         <v>22</v>
       </c>
       <c r="C11" s="2">
-        <v>44621</v>
+        <v>45352</v>
       </c>
       <c r="D11" s="3">
-        <v>44628</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45359</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -798,13 +798,13 @@
         <v>24</v>
       </c>
       <c r="C12" s="3">
-        <v>44628</v>
+        <v>45359</v>
       </c>
       <c r="D12" s="2">
-        <v>44635</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -812,14 +812,14 @@
         <v>26</v>
       </c>
       <c r="C13" s="2">
-        <v>44635</v>
+        <v>45366</v>
       </c>
       <c r="D13" s="2">
-        <v>44642</v>
+        <v>45373</v>
       </c>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -827,13 +827,13 @@
         <v>28</v>
       </c>
       <c r="C14" s="2">
-        <v>44642</v>
+        <v>45373</v>
       </c>
       <c r="D14" s="2">
-        <v>44649</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45380</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -841,13 +841,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="2">
-        <v>44649</v>
+        <v>45380</v>
       </c>
       <c r="D15" s="2">
-        <v>44656</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -855,13 +855,13 @@
         <v>32</v>
       </c>
       <c r="C16" s="2">
-        <v>44656</v>
+        <v>45387</v>
       </c>
       <c r="D16" s="2">
-        <v>44663</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45394</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -869,13 +869,13 @@
         <v>34</v>
       </c>
       <c r="C17" s="2">
-        <v>44663</v>
+        <v>45394</v>
       </c>
       <c r="D17" s="2">
-        <v>44670</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -883,13 +883,13 @@
         <v>36</v>
       </c>
       <c r="C18" s="2">
-        <v>44670</v>
+        <v>45401</v>
       </c>
       <c r="D18" s="2">
-        <v>44677</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45408</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -897,13 +897,13 @@
         <v>38</v>
       </c>
       <c r="C19" s="2">
-        <v>44677</v>
+        <v>45408</v>
       </c>
       <c r="D19" s="2">
-        <v>44684</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -911,13 +911,13 @@
         <v>40</v>
       </c>
       <c r="C20" s="2">
-        <v>44684</v>
+        <v>45415</v>
       </c>
       <c r="D20" s="3">
-        <v>44691</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45422</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -925,13 +925,13 @@
         <v>42</v>
       </c>
       <c r="C21" s="3">
-        <v>44691</v>
+        <v>45422</v>
       </c>
       <c r="D21" s="2">
-        <v>44698</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -939,13 +939,13 @@
         <v>44</v>
       </c>
       <c r="C22" s="2">
-        <v>44698</v>
+        <v>45429</v>
       </c>
       <c r="D22" s="2">
-        <v>44706</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -953,13 +953,13 @@
         <v>5</v>
       </c>
       <c r="C23" s="2">
-        <v>44706</v>
+        <v>45437</v>
       </c>
       <c r="D23" s="2">
-        <v>44572</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -967,13 +967,13 @@
         <v>7</v>
       </c>
       <c r="C24" s="2">
-        <v>44712</v>
+        <v>45443</v>
       </c>
       <c r="D24" s="2">
-        <v>44579</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -981,13 +981,13 @@
         <v>9</v>
       </c>
       <c r="C25" s="2">
-        <v>44719</v>
+        <v>45450</v>
       </c>
       <c r="D25" s="2">
-        <v>44726</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -995,13 +995,13 @@
         <v>11</v>
       </c>
       <c r="C26" s="2">
-        <v>44726</v>
+        <v>45457</v>
       </c>
       <c r="D26" s="2">
-        <v>44733</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1009,13 +1009,13 @@
         <v>13</v>
       </c>
       <c r="C27" s="2">
-        <v>44733</v>
+        <v>45464</v>
       </c>
       <c r="D27" s="2">
-        <v>44740</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -1023,10 +1023,10 @@
         <v>15</v>
       </c>
       <c r="C28" s="2">
-        <v>44740</v>
+        <v>45471</v>
       </c>
       <c r="D28" s="2">
-        <v>44747</v>
+        <v>45478</v>
       </c>
     </row>
   </sheetData>
@@ -1035,4 +1035,10 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
[excel] (Power Automate) Update all articles to use new Power Automate UI (#683)
* Updatng tutorials and some samples

* More partial progress

* All PA samples updated

* Typo fixes

* Add missing image

* Apply suggestions from code review

Co-authored-by: Alison McKay <almckay@microsoft.com>

* Feedback

---------

Co-authored-by: Alison McKay <almckay@microsoft.com>
</commit_message>
<xml_diff>
--- a/docs/tutorials/on-call-rotation.xlsx
+++ b/docs/tutorials/on-call-rotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\office-scripts-docs\docs\tutorials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint-df.com/personal/aljerabe_microsoft_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C310C0E8-66D1-4807-B444-B8B28BFB5CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{C310C0E8-66D1-4807-B444-B8B28BFB5CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E976836-2AF3-4976-98C4-F30870386028}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1" sheetId="1" r:id="rId1"/>
@@ -331,9 +331,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,7 +371,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -477,7 +477,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -630,18 +630,18 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -655,13 +655,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -669,13 +669,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>44565</v>
+        <v>45295</v>
       </c>
       <c r="D3" s="2">
-        <v>44572</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -683,13 +683,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="2">
-        <v>44572</v>
+        <v>45302</v>
       </c>
       <c r="D4" s="2">
-        <v>44579</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -697,13 +697,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="2">
-        <v>44579</v>
+        <v>45309</v>
       </c>
       <c r="D5" s="2">
-        <v>44586</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -711,13 +711,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>44586</v>
+        <v>45316</v>
       </c>
       <c r="D6" s="2">
-        <v>44593</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -725,13 +725,13 @@
         <v>13</v>
       </c>
       <c r="C7" s="2">
-        <v>44593</v>
+        <v>45323</v>
       </c>
       <c r="D7" s="2">
-        <v>44600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -739,13 +739,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="2">
-        <v>44600</v>
+        <v>45330</v>
       </c>
       <c r="D8" s="2">
-        <v>44607</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -753,16 +753,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="2">
-        <v>44607</v>
+        <v>45337</v>
       </c>
       <c r="D9" s="2">
-        <v>44614</v>
+        <v>45344</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -770,13 +770,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="2">
-        <v>44614</v>
+        <v>45344</v>
       </c>
       <c r="D10" s="2">
-        <v>44621</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -784,13 +784,13 @@
         <v>22</v>
       </c>
       <c r="C11" s="2">
-        <v>44621</v>
+        <v>45352</v>
       </c>
       <c r="D11" s="3">
-        <v>44628</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45359</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -798,13 +798,13 @@
         <v>24</v>
       </c>
       <c r="C12" s="3">
-        <v>44628</v>
+        <v>45359</v>
       </c>
       <c r="D12" s="2">
-        <v>44635</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -812,14 +812,14 @@
         <v>26</v>
       </c>
       <c r="C13" s="2">
-        <v>44635</v>
+        <v>45366</v>
       </c>
       <c r="D13" s="2">
-        <v>44642</v>
+        <v>45373</v>
       </c>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -827,13 +827,13 @@
         <v>28</v>
       </c>
       <c r="C14" s="2">
-        <v>44642</v>
+        <v>45373</v>
       </c>
       <c r="D14" s="2">
-        <v>44649</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45380</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -841,13 +841,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="2">
-        <v>44649</v>
+        <v>45380</v>
       </c>
       <c r="D15" s="2">
-        <v>44656</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -855,13 +855,13 @@
         <v>32</v>
       </c>
       <c r="C16" s="2">
-        <v>44656</v>
+        <v>45387</v>
       </c>
       <c r="D16" s="2">
-        <v>44663</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45394</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
@@ -869,13 +869,13 @@
         <v>34</v>
       </c>
       <c r="C17" s="2">
-        <v>44663</v>
+        <v>45394</v>
       </c>
       <c r="D17" s="2">
-        <v>44670</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -883,13 +883,13 @@
         <v>36</v>
       </c>
       <c r="C18" s="2">
-        <v>44670</v>
+        <v>45401</v>
       </c>
       <c r="D18" s="2">
-        <v>44677</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45408</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -897,13 +897,13 @@
         <v>38</v>
       </c>
       <c r="C19" s="2">
-        <v>44677</v>
+        <v>45408</v>
       </c>
       <c r="D19" s="2">
-        <v>44684</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -911,13 +911,13 @@
         <v>40</v>
       </c>
       <c r="C20" s="2">
-        <v>44684</v>
+        <v>45415</v>
       </c>
       <c r="D20" s="3">
-        <v>44691</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45422</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -925,13 +925,13 @@
         <v>42</v>
       </c>
       <c r="C21" s="3">
-        <v>44691</v>
+        <v>45422</v>
       </c>
       <c r="D21" s="2">
-        <v>44698</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -939,13 +939,13 @@
         <v>44</v>
       </c>
       <c r="C22" s="2">
-        <v>44698</v>
+        <v>45429</v>
       </c>
       <c r="D22" s="2">
-        <v>44706</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45437</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -953,13 +953,13 @@
         <v>5</v>
       </c>
       <c r="C23" s="2">
-        <v>44706</v>
+        <v>45437</v>
       </c>
       <c r="D23" s="2">
-        <v>44572</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -967,13 +967,13 @@
         <v>7</v>
       </c>
       <c r="C24" s="2">
-        <v>44712</v>
+        <v>45443</v>
       </c>
       <c r="D24" s="2">
-        <v>44579</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -981,13 +981,13 @@
         <v>9</v>
       </c>
       <c r="C25" s="2">
-        <v>44719</v>
+        <v>45450</v>
       </c>
       <c r="D25" s="2">
-        <v>44726</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45457</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -995,13 +995,13 @@
         <v>11</v>
       </c>
       <c r="C26" s="2">
-        <v>44726</v>
+        <v>45457</v>
       </c>
       <c r="D26" s="2">
-        <v>44733</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
@@ -1009,13 +1009,13 @@
         <v>13</v>
       </c>
       <c r="C27" s="2">
-        <v>44733</v>
+        <v>45464</v>
       </c>
       <c r="D27" s="2">
-        <v>44740</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+        <v>45471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -1023,10 +1023,10 @@
         <v>15</v>
       </c>
       <c r="C28" s="2">
-        <v>44740</v>
+        <v>45471</v>
       </c>
       <c r="D28" s="2">
-        <v>44747</v>
+        <v>45478</v>
       </c>
     </row>
   </sheetData>
@@ -1035,4 +1035,10 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>